<commit_message>
cart plus minus delete
</commit_message>
<xml_diff>
--- a/shop_page/phones_flask_project.xlsx
+++ b/shop_page/phones_flask_project.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Samsung S24 Ultra Titanium</t>
   </si>
   <si>
-    <t xml:space="preserve">64 000 грн</t>
+    <t xml:space="preserve">64000 грн</t>
   </si>
   <si>
     <t xml:space="preserve">256 Гб</t>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Смартфон Samsung Galaxy A35 5G 6/128Gb Awesome Navy</t>
   </si>
   <si>
-    <t xml:space="preserve">14 099 грн</t>
+    <t xml:space="preserve">14099 грн</t>
   </si>
   <si>
     <t xml:space="preserve">128 Гб</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Смартфон Xiaomi Redmi Note 13 Pro 8/256Gb Midnight Black</t>
   </si>
   <si>
-    <t xml:space="preserve">9 999 грн</t>
+    <t xml:space="preserve">9999 грн</t>
   </si>
   <si>
     <t xml:space="preserve">xiaomi-redmi-note-13-pro.jpg</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Мобільний телефон Oppo A78 8/256GB</t>
   </si>
   <si>
-    <t xml:space="preserve">10 232 грн</t>
+    <t xml:space="preserve">10232 грн</t>
   </si>
   <si>
     <t xml:space="preserve">oppo-a78.jpg</t>
@@ -282,18 +282,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -312,6 +312,9 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="0" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -329,6 +332,9 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F2" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -346,6 +352,9 @@
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -363,6 +372,9 @@
       <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F4" s="0" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
@@ -379,6 +391,9 @@
       </c>
       <c r="E5" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>